<commit_message>
the cell replace engine for dungeon story
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/DungeonStory.xlsx
+++ b/ConfigData/Xlsx/DungeonStory.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -131,13 +131,29 @@
   </si>
   <si>
     <t>所有的敌人等级+1|所有的怪死亡</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>替换</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EventReplace</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bossqiongqi=bossunicorn</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -335,7 +351,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -537,6 +553,18 @@
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor theme="4"/>
       </patternFill>
     </fill>
   </fills>
@@ -804,7 +832,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -845,6 +873,15 @@
       <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -892,7 +929,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="12">
     <dxf>
       <font>
         <b val="0"/>
@@ -911,16 +948,6 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -959,6 +986,35 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1176,17 +1232,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:H5" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8">
-  <autoFilter ref="A3:H5"/>
-  <tableColumns count="8">
-    <tableColumn id="1" name="Id" dataDxfId="7"/>
-    <tableColumn id="2" name="Name" dataDxfId="6"/>
-    <tableColumn id="3" name="Descript" dataDxfId="5"/>
-    <tableColumn id="24" name="RuleStr" dataDxfId="0"/>
-    <tableColumn id="6" name="Rate" dataDxfId="4"/>
-    <tableColumn id="9" name="DungeonId" dataDxfId="3"/>
-    <tableColumn id="16" name="NeedGismoId" dataDxfId="2"/>
-    <tableColumn id="4" name="Image" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:I5" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9">
+  <autoFilter ref="A3:I5" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Descript" dataDxfId="6"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="RuleStr" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Rate" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="DungeonId" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="NeedGismoId" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{A347D9D0-C79A-41A5-91ED-B8BDE1173C73}" name="EventReplace" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Image" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1512,11 +1569,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1527,11 +1584,12 @@
     <col min="5" max="5" width="5.625" style="3" customWidth="1"/>
     <col min="6" max="6" width="9.5" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="9.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="3"/>
+    <col min="8" max="8" width="26.125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1553,11 +1611,14 @@
       <c r="G1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1579,11 +1640,14 @@
       <c r="G2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1605,11 +1669,14 @@
       <c r="G3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="7">
         <v>47000001</v>
       </c>
@@ -1627,11 +1694,12 @@
         <v>18000001</v>
       </c>
       <c r="G4" s="10"/>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="10"/>
+      <c r="I4" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="7">
         <v>47000002</v>
       </c>
@@ -1654,6 +1722,9 @@
         <v>45000001</v>
       </c>
       <c r="H5" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="10" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
optimise the story form
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/DungeonStory.xlsx
+++ b/ConfigData/Xlsx/DungeonStory.xlsx
@@ -130,10 +130,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>所有的敌人等级+1|所有的怪死亡</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>替换</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -146,7 +142,11 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>bossqiongqi=bossunicorn</t>
+    <t>bossqiongqi=bossunicorn,manflower=wolfnest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>会出现一些狼群|所有的怪死亡</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1612,7 +1612,7 @@
         <v>18</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>22</v>
@@ -1641,7 +1641,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>3</v>
@@ -1670,7 +1670,7 @@
         <v>19</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>17</v>
@@ -1710,7 +1710,7 @@
         <v>21</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E5" s="8">
         <v>50</v>
@@ -1722,7 +1722,7 @@
         <v>45000001</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I5" s="10" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
add some story addon func
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/DungeonStory.xlsx
+++ b/ConfigData/Xlsx/DungeonStory.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -104,10 +104,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>找到传说中的神兽【独角兽】，并击败它</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>背景图</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -146,7 +142,39 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>会出现一些狼群|所有的怪死亡</t>
+    <t>主鉴定</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>主鉴定修正</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>intl</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttrType</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttrBias</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>额外卡牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CardId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>会出现一些狼群|智慧属性下降1点|额外获得一张卡牌【侏儒】</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过【侏儒】的引导，找到传说中的神兽【独角兽】</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -351,7 +379,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -567,8 +595,20 @@
         <bgColor theme="4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -703,6 +743,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -832,7 +881,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -883,6 +932,15 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -929,7 +987,92 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1232,18 +1375,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:I5" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9">
-  <autoFilter ref="A3:I5" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Descript" dataDxfId="6"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="RuleStr" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Rate" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="DungeonId" dataDxfId="3"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="NeedGismoId" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{A347D9D0-C79A-41A5-91ED-B8BDE1173C73}" name="EventReplace" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Image" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:L5" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16">
+  <autoFilter ref="A3:L5" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Descript" dataDxfId="13"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="RuleStr" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Rate" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="DungeonId" dataDxfId="10"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="NeedGismoId" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{A347D9D0-C79A-41A5-91ED-B8BDE1173C73}" name="EventReplace" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{B2A337FE-0C24-4460-B3AD-B636612A7844}" name="AttrType" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{E0489051-D594-4CA6-BFC1-454DA9F2CB87}" name="AttrBias" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{F9CC78E4-7B84-4315-B48E-4BDEC60226B0}" name="CardId" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Image" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1570,10 +1716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1585,11 +1731,13 @@
     <col min="6" max="6" width="9.5" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.125" style="3" customWidth="1"/>
     <col min="8" max="8" width="26.125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="9.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="3"/>
+    <col min="9" max="10" width="5.875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="9.625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1600,7 +1748,7 @@
         <v>15</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>12</v>
@@ -1612,13 +1760,22 @@
         <v>18</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1629,7 +1786,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>11</v>
@@ -1641,13 +1798,22 @@
         <v>0</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="17" t="s">
         <v>3</v>
       </c>
+      <c r="J2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1658,7 +1824,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>13</v>
@@ -1670,13 +1836,22 @@
         <v>19</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4" s="7">
         <v>47000001</v>
       </c>
@@ -1695,11 +1870,14 @@
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
-      <c r="I4" s="10" t="s">
-        <v>23</v>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A5" s="7">
         <v>47000002</v>
       </c>
@@ -1707,13 +1885,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="E5" s="8">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="F5" s="8">
         <v>18000001</v>
@@ -1722,14 +1900,33 @@
         <v>45000001</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>24</v>
+        <v>33</v>
+      </c>
+      <c r="J5" s="10">
+        <v>-1</v>
+      </c>
+      <c r="K5" s="10">
+        <v>51000046</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
+  <conditionalFormatting sqref="G4:J5 L4:L5">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(G4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4:K5">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
+      <formula>LEN(TRIM(K4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
support bless for dungeon story
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/DungeonStory.xlsx
+++ b/ConfigData/Xlsx/DungeonStory.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -175,13 +175,21 @@
   </si>
   <si>
     <t>通过【侏儒】的引导，找到传说中的神兽【独角兽】</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>额外祝福</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BlessId</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1029,11 +1037,23 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1363,6 +1383,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1375,21 +1463,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:L5" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16">
-  <autoFilter ref="A3:L5" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Descript" dataDxfId="13"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="RuleStr" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Rate" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="DungeonId" dataDxfId="10"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="NeedGismoId" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{A347D9D0-C79A-41A5-91ED-B8BDE1173C73}" name="EventReplace" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{B2A337FE-0C24-4460-B3AD-B636612A7844}" name="AttrType" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{E0489051-D594-4CA6-BFC1-454DA9F2CB87}" name="AttrBias" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{F9CC78E4-7B84-4315-B48E-4BDEC60226B0}" name="CardId" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Image" dataDxfId="5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:M5" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16">
+  <autoFilter ref="A3:M5"/>
+  <tableColumns count="13">
+    <tableColumn id="1" name="Id" dataDxfId="15"/>
+    <tableColumn id="2" name="Name" dataDxfId="14"/>
+    <tableColumn id="3" name="Descript" dataDxfId="13"/>
+    <tableColumn id="24" name="RuleStr" dataDxfId="12"/>
+    <tableColumn id="6" name="Rate" dataDxfId="11"/>
+    <tableColumn id="9" name="DungeonId" dataDxfId="10"/>
+    <tableColumn id="16" name="NeedGismoId" dataDxfId="9"/>
+    <tableColumn id="5" name="EventReplace" dataDxfId="8"/>
+    <tableColumn id="8" name="AttrType" dataDxfId="7"/>
+    <tableColumn id="7" name="AttrBias" dataDxfId="6"/>
+    <tableColumn id="10" name="CardId" dataDxfId="5"/>
+    <tableColumn id="11" name="BlessId" dataDxfId="0"/>
+    <tableColumn id="4" name="Image" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1403,7 +1492,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1715,11 +1804,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1732,12 +1821,12 @@
     <col min="7" max="7" width="9.125" style="3" customWidth="1"/>
     <col min="8" max="8" width="26.125" style="3" customWidth="1"/>
     <col min="9" max="10" width="5.875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="9.625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="9.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="3"/>
+    <col min="11" max="12" width="9.625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1771,11 +1860,14 @@
       <c r="K1" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1809,11 +1901,14 @@
       <c r="K2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1847,11 +1942,14 @@
       <c r="K3" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="L3" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4" s="7">
         <v>47000001</v>
       </c>
@@ -1873,11 +1971,12 @@
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="10"/>
+      <c r="M4" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5" s="7">
         <v>47000002</v>
       </c>
@@ -1911,20 +2010,26 @@
       <c r="K5" s="10">
         <v>51000046</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="10"/>
+      <c r="M5" s="10" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="G4:J5 L4:L5">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
+  <conditionalFormatting sqref="G4:J5 M4:M5">
+    <cfRule type="containsBlanks" dxfId="3" priority="4">
       <formula>LEN(TRIM(G4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:K5">
+    <cfRule type="containsBlanks" dxfId="2" priority="2">
+      <formula>LEN(TRIM(K4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L4:L5">
     <cfRule type="containsBlanks" dxfId="1" priority="1">
-      <formula>LEN(TRIM(K4))=0</formula>
+      <formula>LEN(TRIM(L4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ColorLabel support auto new label and border enhancement
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/DungeonStory.xlsx
+++ b/ConfigData/Xlsx/DungeonStory.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -84,10 +84,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>找到传说中的神兽【穷奇】，并击败它</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Image</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -110,7 +106,7 @@
     <t>unicorn</t>
   </si>
   <si>
-    <t>规则说明</t>
+    <t>替换</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -118,18 +114,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>RuleStr</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>替换</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>EventReplace</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -166,14 +150,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>会出现一些狼群|智慧属性下降1点|额外获得一张卡牌【侏儒】</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>通过【侏儒】的引导，找到传说中的神兽【独角兽】</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>额外祝福</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -186,14 +162,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>找到迷宫出口</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>充满了很多机关|找到出口异常艰辛</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>lost</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -211,6 +179,18 @@
   </si>
   <si>
     <t>NeedGismoId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>找到传说中的神兽【穷奇】，并击败它找到传说中的神兽【穷奇】，并击败它找到传说中的神兽【穷奇】，并击败它找到传说中的神兽【穷奇】，并击败它找到传说中的神兽【穷奇】，并击败它\n会出现一些狼群\nGreen|智慧属性下降1点\n额外获得一张卡牌【侏儒】</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过【侏儒】的引导，找到传说中的神兽【独角兽】\nLime|会出现一些狼群\nLime|智慧属性下降1点\nLime|额外获得一张卡牌【侏儒】</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>找到迷宫出口\nLime|充满了很多机关\nLime|找到出口异常艰辛</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1023,7 +1003,35 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1322,35 +1330,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <left style="thin">
           <color theme="4"/>
@@ -1407,36 +1386,76 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1449,23 +1468,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:N6" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" tableBorderDxfId="14">
-  <autoFilter ref="A3:N6"/>
-  <tableColumns count="14">
-    <tableColumn id="1" name="Id" dataDxfId="13"/>
-    <tableColumn id="2" name="Name" dataDxfId="12"/>
-    <tableColumn id="3" name="Descript" dataDxfId="11"/>
-    <tableColumn id="24" name="RuleStr" dataDxfId="10"/>
-    <tableColumn id="6" name="Rate" dataDxfId="9"/>
-    <tableColumn id="9" name="DungeonId" dataDxfId="8"/>
-    <tableColumn id="12" name="NeedLevel" dataDxfId="7"/>
-    <tableColumn id="16" name="NeedGismoId" dataDxfId="6"/>
-    <tableColumn id="5" name="EventReplace" dataDxfId="5"/>
-    <tableColumn id="8" name="AttrType" dataDxfId="4"/>
-    <tableColumn id="7" name="AttrBias" dataDxfId="3"/>
-    <tableColumn id="10" name="CardId" dataDxfId="2"/>
-    <tableColumn id="11" name="BlessId" dataDxfId="1"/>
-    <tableColumn id="4" name="Image" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:M6" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17">
+  <autoFilter ref="A3:M6"/>
+  <tableColumns count="13">
+    <tableColumn id="1" name="Id" dataDxfId="16"/>
+    <tableColumn id="2" name="Name" dataDxfId="15"/>
+    <tableColumn id="3" name="Descript" dataDxfId="14"/>
+    <tableColumn id="6" name="Rate" dataDxfId="13"/>
+    <tableColumn id="9" name="DungeonId" dataDxfId="12"/>
+    <tableColumn id="12" name="NeedLevel" dataDxfId="11"/>
+    <tableColumn id="16" name="NeedGismoId" dataDxfId="10"/>
+    <tableColumn id="5" name="EventReplace" dataDxfId="9"/>
+    <tableColumn id="8" name="AttrType" dataDxfId="8"/>
+    <tableColumn id="7" name="AttrBias" dataDxfId="7"/>
+    <tableColumn id="10" name="CardId" dataDxfId="6"/>
+    <tableColumn id="11" name="BlessId" dataDxfId="5"/>
+    <tableColumn id="4" name="Image" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1479,7 +1497,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1792,29 +1810,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.5" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="3"/>
-    <col min="3" max="4" width="26.125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="5.625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="9.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5" style="3" customWidth="1"/>
-    <col min="8" max="8" width="9.5" style="3" customWidth="1"/>
-    <col min="9" max="9" width="26.125" style="3" customWidth="1"/>
-    <col min="10" max="11" width="5.875" style="3" customWidth="1"/>
-    <col min="12" max="13" width="9.625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="9.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9" style="3"/>
+    <col min="3" max="3" width="26.125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="5.625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.5" style="3" customWidth="1"/>
+    <col min="8" max="8" width="26.125" style="3" customWidth="1"/>
+    <col min="9" max="10" width="5.875" style="3" customWidth="1"/>
+    <col min="11" max="12" width="9.625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1825,40 +1843,37 @@
         <v>15</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="F1" s="12" t="s">
+        <v>39</v>
+      </c>
       <c r="G1" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="19" t="s">
         <v>26</v>
       </c>
       <c r="J1" s="19" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K1" s="19" t="s">
         <v>31</v>
       </c>
       <c r="L1" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>20</v>
+        <v>33</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1869,25 +1884,25 @@
         <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="5" t="s">
         <v>4</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>0</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="17" t="s">
         <v>0</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>3</v>
       </c>
       <c r="K2" s="17" t="s">
         <v>0</v>
@@ -1895,14 +1910,11 @@
       <c r="L2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="M2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="N2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1913,40 +1925,37 @@
         <v>10</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="9" t="s">
         <v>7</v>
       </c>
+      <c r="F3" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="G3" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" s="16" t="s">
-        <v>28</v>
+        <v>40</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>29</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K3" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="M3" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>17</v>
+      <c r="M3" s="9" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4" s="7">
         <v>47000001</v>
       </c>
@@ -1954,120 +1963,113 @@
         <v>14</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="8"/>
+        <v>41</v>
+      </c>
+      <c r="D4" s="8">
+        <v>100</v>
+      </c>
       <c r="E4" s="8">
-        <v>100</v>
-      </c>
-      <c r="F4" s="8">
         <v>18000001</v>
       </c>
+      <c r="F4" s="10"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10" t="s">
-        <v>21</v>
+      <c r="M4" s="10" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5" s="7">
         <v>47000002</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="D5" s="8">
+        <v>70</v>
       </c>
       <c r="E5" s="8">
-        <v>70</v>
-      </c>
-      <c r="F5" s="8">
         <v>18000001</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10">
+      <c r="F5" s="10"/>
+      <c r="G5" s="10">
         <v>45000001</v>
       </c>
+      <c r="H5" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="I5" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+      <c r="J5" s="10">
+        <v>-1</v>
       </c>
       <c r="K5" s="10">
-        <v>-1</v>
-      </c>
-      <c r="L5" s="10">
         <v>51000046</v>
       </c>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10" t="s">
-        <v>22</v>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A6" s="7">
         <v>47000003</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="8" t="s">
         <v>43</v>
       </c>
+      <c r="D6" s="8">
+        <v>60</v>
+      </c>
       <c r="E6" s="8">
-        <v>60</v>
-      </c>
-      <c r="F6" s="8">
         <v>18000001</v>
       </c>
-      <c r="G6" s="10">
+      <c r="F6" s="10">
         <v>5</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10" t="s">
-        <v>45</v>
-      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="10"/>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
       <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10" t="s">
-        <v>44</v>
+      <c r="M6" s="10" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="H4:K6 N4:N6">
-    <cfRule type="containsBlanks" dxfId="20" priority="5">
-      <formula>LEN(TRIM(H4))=0</formula>
+  <conditionalFormatting sqref="G4:J6 M4:M6">
+    <cfRule type="containsBlanks" dxfId="3" priority="5">
+      <formula>LEN(TRIM(G4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4:K6">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(K4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:L6">
-    <cfRule type="containsBlanks" dxfId="19" priority="3">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(L4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M4:M6">
-    <cfRule type="containsBlanks" dxfId="18" priority="2">
-      <formula>LEN(TRIM(M4))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G6">
-    <cfRule type="containsBlanks" dxfId="17" priority="1">
-      <formula>LEN(TRIM(G4))=0</formula>
+  <conditionalFormatting sqref="F4:F6">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(F4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update the colorlabel text format
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/DungeonStory.xlsx
+++ b/ConfigData/Xlsx/DungeonStory.xlsx
@@ -182,15 +182,15 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>找到传说中的神兽【穷奇】，并击败它找到传说中的神兽【穷奇】，并击败它找到传说中的神兽【穷奇】，并击败它找到传说中的神兽【穷奇】，并击败它找到传说中的神兽【穷奇】，并击败它\n会出现一些狼群\nGreen|智慧属性下降1点\n额外获得一张卡牌【侏儒】</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>通过【侏儒】的引导，找到传说中的神兽【独角兽】\nLime|会出现一些狼群\nLime|智慧属性下降1点\nLime|额外获得一张卡牌【侏儒】</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>找到迷宫出口\nLime|充满了很多机关\nLime|找到出口异常艰辛</t>
+    <t>穷奇，中国神话传说中的古代四凶之一。记载于《山海经》中，指穷奇外貌像老虎，长有一双翅膀，喜欢吃人，更会从人的头部开始进食，是一头凶恶的异兽。|n|最近有村民发现该神兽在森林中出现，你的任务是|#ff6666|尝试寻找并杀死传说中的神兽【穷奇】||，使森林重新归于平静。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过【侏儒】的引导，找到传说中的神兽【独角兽】|n#66ff66|会出现一些狼群|n#66ff66|智慧属性下降1点|n#66ff66|额外获得一张卡牌【侏儒】</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>找到迷宫出口|n#66ff66|充满了很多机关|n#66ff66|找到出口异常艰辛</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1004,34 +1004,6 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="20">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1386,6 +1358,34 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1468,22 +1468,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:M6" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:M6" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="13">
   <autoFilter ref="A3:M6"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="Id" dataDxfId="16"/>
-    <tableColumn id="2" name="Name" dataDxfId="15"/>
-    <tableColumn id="3" name="Descript" dataDxfId="14"/>
-    <tableColumn id="6" name="Rate" dataDxfId="13"/>
-    <tableColumn id="9" name="DungeonId" dataDxfId="12"/>
-    <tableColumn id="12" name="NeedLevel" dataDxfId="11"/>
-    <tableColumn id="16" name="NeedGismoId" dataDxfId="10"/>
-    <tableColumn id="5" name="EventReplace" dataDxfId="9"/>
-    <tableColumn id="8" name="AttrType" dataDxfId="8"/>
-    <tableColumn id="7" name="AttrBias" dataDxfId="7"/>
-    <tableColumn id="10" name="CardId" dataDxfId="6"/>
-    <tableColumn id="11" name="BlessId" dataDxfId="5"/>
-    <tableColumn id="4" name="Image" dataDxfId="4"/>
+    <tableColumn id="1" name="Id" dataDxfId="12"/>
+    <tableColumn id="2" name="Name" dataDxfId="11"/>
+    <tableColumn id="3" name="Descript" dataDxfId="10"/>
+    <tableColumn id="6" name="Rate" dataDxfId="9"/>
+    <tableColumn id="9" name="DungeonId" dataDxfId="8"/>
+    <tableColumn id="12" name="NeedLevel" dataDxfId="7"/>
+    <tableColumn id="16" name="NeedGismoId" dataDxfId="6"/>
+    <tableColumn id="5" name="EventReplace" dataDxfId="5"/>
+    <tableColumn id="8" name="AttrType" dataDxfId="4"/>
+    <tableColumn id="7" name="AttrBias" dataDxfId="3"/>
+    <tableColumn id="10" name="CardId" dataDxfId="2"/>
+    <tableColumn id="11" name="BlessId" dataDxfId="1"/>
+    <tableColumn id="4" name="Image" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1813,7 +1813,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2053,22 +2053,22 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="G4:J6 M4:M6">
-    <cfRule type="containsBlanks" dxfId="3" priority="5">
+    <cfRule type="containsBlanks" dxfId="19" priority="5">
       <formula>LEN(TRIM(G4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:K6">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
+    <cfRule type="containsBlanks" dxfId="18" priority="3">
       <formula>LEN(TRIM(K4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:L6">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+    <cfRule type="containsBlanks" dxfId="17" priority="2">
       <formula>LEN(TRIM(L4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:F6">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="16" priority="1">
       <formula>LEN(TRIM(F4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>